<commit_message>
edit muting rules spreadsheet
</commit_message>
<xml_diff>
--- a/Muting Rules.xlsx
+++ b/Muting Rules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeversmeyer\Muting Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://2ndwatch-my.sharepoint.com/personal/aeversmeyer_2ndwatch_com/Documents/Documents/Tooling/NR Muting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDEF409-76FC-4A6C-9AD2-28A36C44CA24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="717" documentId="8_{F3C4CCFD-D3A3-4A0C-A232-E9C71F11B485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0463F129-B798-4DF9-9E3B-A1CA3351B187}"/>
   <bookViews>
-    <workbookView xWindow="38310" yWindow="2310" windowWidth="37680" windowHeight="16840" xr2:uid="{D6AE10F8-5FA4-4DCC-834E-28D78D72E9DB}"/>
+    <workbookView xWindow="470" yWindow="1700" windowWidth="37680" windowHeight="16840" xr2:uid="{D6AE10F8-5FA4-4DCC-834E-28D78D72E9DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="197">
   <si>
     <t>Environment</t>
   </si>
@@ -197,21 +197,6 @@
     <t>linux instances patched quarterly, same tag</t>
   </si>
   <si>
-    <t>NP ECS</t>
-  </si>
-  <si>
-    <t>NP App, IIS, SQL grp 3</t>
-  </si>
-  <si>
-    <t>Prod Azure</t>
-  </si>
-  <si>
-    <t>Prod App, IIS, SQL grp 3</t>
-  </si>
-  <si>
-    <t>Prod ECS</t>
-  </si>
-  <si>
     <t>Prod_ECS_Group_1</t>
   </si>
   <si>
@@ -266,18 +251,6 @@
     <t>Prod_SQL_Group_3</t>
   </si>
   <si>
-    <t>Prod App, Infra, SQL grp 1</t>
-  </si>
-  <si>
-    <t>Prod App, Infra, SQL grp 2</t>
-  </si>
-  <si>
-    <t>NP App, SQL grp 1</t>
-  </si>
-  <si>
-    <t>NP App, SQL grp 2</t>
-  </si>
-  <si>
     <t>prod-linux</t>
   </si>
   <si>
@@ -398,9 +371,6 @@
     <t>Cypherworx</t>
   </si>
   <si>
-    <t>GreenFirst Forest Products</t>
-  </si>
-  <si>
     <t>CKE Restaurants</t>
   </si>
   <si>
@@ -627,6 +597,36 @@
   </si>
   <si>
     <t>Prod_Linux_Quarterly-M1_Thur-W3</t>
+  </si>
+  <si>
+    <t>Non-Prod -Infra and SQL group2</t>
+  </si>
+  <si>
+    <t>Non-Prod -App, IIS and SQL group3</t>
+  </si>
+  <si>
+    <t>Non-Prod - ECS</t>
+  </si>
+  <si>
+    <t>Prod -App, IIS and SQL group3</t>
+  </si>
+  <si>
+    <t>Prod - App,Prod-Infra Group 1, and SQL group1</t>
+  </si>
+  <si>
+    <t>Prod -App,Prod -Infra Group 2, and SQL group2</t>
+  </si>
+  <si>
+    <t>Prod - Azure</t>
+  </si>
+  <si>
+    <t>Prod - ECS</t>
+  </si>
+  <si>
+    <t>Non-Prod - App and SQL group1</t>
+  </si>
+  <si>
+    <t>GreenFirst Forsest Products</t>
   </si>
 </sst>
 </file>
@@ -762,6 +762,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1063,14 +1067,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5344475A-C7FB-4B36-9EFD-5513E556E893}">
   <dimension ref="A1:O81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.453125" customWidth="1"/>
-    <col min="2" max="2" width="23.08984375" customWidth="1"/>
+    <col min="2" max="2" width="40.26953125" customWidth="1"/>
     <col min="3" max="3" width="20.90625" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="35.36328125" customWidth="1"/>
@@ -1097,40 +1101,40 @@
         <v>32</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
@@ -1138,7 +1142,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>31</v>
@@ -1147,17 +1151,17 @@
         <v>7</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="L2" s="11">
         <v>38494683</v>
@@ -1167,7 +1171,7 @@
       </c>
       <c r="N2" s="10"/>
       <c r="O2" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
@@ -1175,7 +1179,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>31</v>
@@ -1184,17 +1188,17 @@
         <v>7</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="L3" s="11">
         <v>38494726</v>
@@ -1204,7 +1208,7 @@
       </c>
       <c r="N3" s="10"/>
       <c r="O3" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
@@ -1212,7 +1216,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>31</v>
@@ -1221,17 +1225,17 @@
         <v>7</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="L4" s="11">
         <v>38494771</v>
@@ -1241,7 +1245,7 @@
       </c>
       <c r="N4" s="10"/>
       <c r="O4" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
@@ -1249,7 +1253,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>31</v>
@@ -1258,17 +1262,17 @@
         <v>7</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="L5" s="11">
         <v>38494810</v>
@@ -1278,7 +1282,7 @@
       </c>
       <c r="N5" s="10"/>
       <c r="O5" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
@@ -1286,7 +1290,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>31</v>
@@ -1295,17 +1299,17 @@
         <v>7</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="L6" s="11">
         <v>38494883</v>
@@ -1315,7 +1319,7 @@
       </c>
       <c r="N6" s="10"/>
       <c r="O6" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
@@ -1323,7 +1327,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>31</v>
@@ -1332,17 +1336,17 @@
         <v>7</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="L7" s="11">
         <v>38494924</v>
@@ -1352,7 +1356,7 @@
       </c>
       <c r="N7" s="10"/>
       <c r="O7" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
@@ -1360,7 +1364,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>31</v>
@@ -1369,17 +1373,17 @@
         <v>7</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="L8" s="11">
         <v>38494972</v>
@@ -1389,7 +1393,7 @@
       </c>
       <c r="N8" s="10"/>
       <c r="O8" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
@@ -1397,7 +1401,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>31</v>
@@ -1406,17 +1410,17 @@
         <v>7</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="L9" s="11">
         <v>38495019</v>
@@ -1426,7 +1430,7 @@
       </c>
       <c r="N9" s="10"/>
       <c r="O9" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
@@ -1434,7 +1438,7 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D10" t="s">
         <v>34</v>
@@ -1455,7 +1459,7 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D11" t="s">
         <v>34</v>
@@ -1473,17 +1477,17 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -1502,17 +1506,17 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
@@ -1534,7 +1538,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>54</v>
+        <v>188</v>
       </c>
       <c r="C14" t="s">
         <v>31</v>
@@ -1543,13 +1547,13 @@
         <v>34</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="G14" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -1568,7 +1572,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>78</v>
+        <v>195</v>
       </c>
       <c r="C15" t="s">
         <v>31</v>
@@ -1577,10 +1581,10 @@
         <v>34</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -1600,7 +1604,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>79</v>
+        <v>187</v>
       </c>
       <c r="C16" t="s">
         <v>31</v>
@@ -1609,10 +1613,10 @@
         <v>34</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="L16" s="2">
         <v>38491476</v>
@@ -1627,7 +1631,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>53</v>
+        <v>189</v>
       </c>
       <c r="C17" t="s">
         <v>31</v>
@@ -1636,7 +1640,7 @@
         <v>34</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -1657,7 +1661,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>56</v>
+        <v>190</v>
       </c>
       <c r="C18" t="s">
         <v>31</v>
@@ -1666,13 +1670,13 @@
         <v>34</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -1691,7 +1695,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>76</v>
+        <v>191</v>
       </c>
       <c r="C19" t="s">
         <v>31</v>
@@ -1700,13 +1704,13 @@
         <v>34</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -1725,7 +1729,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>77</v>
+        <v>192</v>
       </c>
       <c r="C20" t="s">
         <v>31</v>
@@ -1734,13 +1738,13 @@
         <v>34</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -1759,7 +1763,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>55</v>
+        <v>193</v>
       </c>
       <c r="C21" t="s">
         <v>31</v>
@@ -1768,7 +1772,7 @@
         <v>34</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="L21" s="2">
         <v>38491356</v>
@@ -1777,7 +1781,7 @@
         <v>2622938</v>
       </c>
       <c r="N21" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
@@ -1785,7 +1789,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>57</v>
+        <v>194</v>
       </c>
       <c r="C22" t="s">
         <v>31</v>
@@ -1794,7 +1798,7 @@
         <v>34</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -1815,7 +1819,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10" t="s">
@@ -1844,7 +1848,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10" t="s">
@@ -1870,10 +1874,10 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B25" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D25" t="s">
         <v>34</v>
@@ -1891,10 +1895,10 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D26" t="s">
         <v>34</v>
@@ -1915,7 +1919,7 @@
         <v>15</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10" t="s">
@@ -1944,7 +1948,7 @@
         <v>15</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10" t="s">
@@ -1973,7 +1977,7 @@
         <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D29" t="s">
         <v>34</v>
@@ -1994,7 +1998,7 @@
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D30" t="s">
         <v>34</v>
@@ -2012,10 +2016,10 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>120</v>
+        <v>196</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9" t="s">
@@ -2037,18 +2041,18 @@
         <v>3169165</v>
       </c>
       <c r="N31" s="10" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="O31" s="10" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>120</v>
+        <v>196</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9" t="s">
@@ -2070,27 +2074,27 @@
         <v>3169165</v>
       </c>
       <c r="N32" s="10" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="O32" s="10" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B33" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
         <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E33" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="L33" s="2">
         <v>38495239</v>
@@ -2102,19 +2106,19 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B34" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C34" t="s">
         <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E34" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="L34" s="2">
         <v>38495273</v>
@@ -2126,25 +2130,25 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C35" t="s">
         <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E35" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F35" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="G35" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="L35" s="2">
         <v>38495325</v>
@@ -2159,7 +2163,7 @@
         <v>26</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10" t="s">
@@ -2190,7 +2194,7 @@
         <v>26</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10" t="s">
@@ -2219,7 +2223,7 @@
         <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D38" t="s">
         <v>34</v>
@@ -2236,7 +2240,7 @@
         <v>27</v>
       </c>
       <c r="B39" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D39" t="s">
         <v>34</v>
@@ -2259,19 +2263,19 @@
         <v>11</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
@@ -2285,10 +2289,10 @@
         <v>2709551</v>
       </c>
       <c r="N40" s="9" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="O40" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.35">
@@ -2296,19 +2300,19 @@
         <v>11</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
@@ -2322,10 +2326,10 @@
         <v>2709551</v>
       </c>
       <c r="N41" s="9" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="O41" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.35">
@@ -2333,14 +2337,14 @@
         <v>3</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -2353,7 +2357,7 @@
         <v>2726091</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="O42" s="4"/>
     </row>
@@ -2369,7 +2373,7 @@
         <v>34</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -2382,7 +2386,7 @@
         <v>2726091</v>
       </c>
       <c r="N43" s="4" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="O43" s="4"/>
     </row>
@@ -2391,14 +2395,14 @@
         <v>3</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -2411,10 +2415,10 @@
         <v>2726091</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="O44" s="4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.35">
@@ -2422,16 +2426,16 @@
         <v>21</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
@@ -2447,7 +2451,7 @@
       </c>
       <c r="N45" s="10"/>
       <c r="O45" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.35">
@@ -2455,16 +2459,16 @@
         <v>21</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C46" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
@@ -2480,7 +2484,7 @@
       </c>
       <c r="N46" s="10"/>
       <c r="O46" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.35">
@@ -2488,16 +2492,16 @@
         <v>21</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
@@ -2513,7 +2517,7 @@
       </c>
       <c r="N47" s="10"/>
       <c r="O47" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.35">
@@ -2521,16 +2525,16 @@
         <v>21</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
@@ -2546,7 +2550,7 @@
       </c>
       <c r="N48" s="10"/>
       <c r="O48" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.35">
@@ -2554,16 +2558,16 @@
         <v>21</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
@@ -2579,7 +2583,7 @@
       </c>
       <c r="N49" s="10"/>
       <c r="O49" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.35">
@@ -2587,7 +2591,7 @@
         <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D50" t="s">
         <v>28</v>
@@ -2608,7 +2612,7 @@
         <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D51" t="s">
         <v>28</v>
@@ -2629,7 +2633,7 @@
         <v>16</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10" t="s">
@@ -2658,7 +2662,7 @@
         <v>16</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C53" s="10"/>
       <c r="D53" s="10" t="s">
@@ -2687,7 +2691,7 @@
         <v>17</v>
       </c>
       <c r="B54" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D54" t="s">
         <v>28</v>
@@ -2708,7 +2712,7 @@
         <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D55" t="s">
         <v>28</v>
@@ -2729,16 +2733,16 @@
         <v>24</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
@@ -2760,19 +2764,19 @@
         <v>24</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="G57" s="10"/>
       <c r="H57" s="10"/>
@@ -2793,19 +2797,19 @@
         <v>12</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C58" t="s">
         <v>31</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="L58" s="2">
         <v>38493910</v>
@@ -2820,22 +2824,22 @@
         <v>12</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C59" t="s">
         <v>31</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
@@ -2854,19 +2858,19 @@
         <v>12</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C60" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="L60" s="2">
         <v>38493945</v>
@@ -2878,22 +2882,22 @@
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G61" s="10"/>
       <c r="H61" s="10"/>
@@ -2903,71 +2907,71 @@
       <c r="L61" s="11"/>
       <c r="M61" s="11"/>
       <c r="N61" s="10" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="O61" s="10"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C62" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="H62" s="10" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="I62" s="10" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="J62" s="10"/>
       <c r="K62" s="10"/>
       <c r="L62" s="11"/>
       <c r="M62" s="11"/>
       <c r="N62" s="10" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="O62" s="10"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B63" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="G63" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="C63" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="G63" s="10" t="s">
-        <v>170</v>
-      </c>
       <c r="H63" s="10" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="I63" s="10"/>
       <c r="J63" s="10"/>
@@ -2975,7 +2979,7 @@
       <c r="L63" s="11"/>
       <c r="M63" s="11"/>
       <c r="N63" s="10" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="O63" s="10"/>
     </row>
@@ -2984,7 +2988,7 @@
         <v>25</v>
       </c>
       <c r="B64" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D64" t="s">
         <v>34</v>
@@ -3005,7 +3009,7 @@
         <v>25</v>
       </c>
       <c r="B65" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D65" t="s">
         <v>34</v>
@@ -3023,10 +3027,10 @@
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C66" s="9"/>
       <c r="D66" s="9" t="s">
@@ -3057,7 +3061,7 @@
         <v>18</v>
       </c>
       <c r="B67" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C67" t="s">
         <v>31</v>
@@ -3066,7 +3070,7 @@
         <v>34</v>
       </c>
       <c r="E67" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="L67" s="2">
         <v>38507716</v>
@@ -3081,22 +3085,22 @@
         <v>18</v>
       </c>
       <c r="B68" t="s">
+        <v>164</v>
+      </c>
+      <c r="C68" t="s">
+        <v>31</v>
+      </c>
+      <c r="D68" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68" t="s">
+        <v>169</v>
+      </c>
+      <c r="F68" t="s">
+        <v>173</v>
+      </c>
+      <c r="G68" t="s">
         <v>174</v>
-      </c>
-      <c r="C68" t="s">
-        <v>31</v>
-      </c>
-      <c r="D68" t="s">
-        <v>34</v>
-      </c>
-      <c r="E68" t="s">
-        <v>179</v>
-      </c>
-      <c r="F68" t="s">
-        <v>183</v>
-      </c>
-      <c r="G68" t="s">
-        <v>184</v>
       </c>
       <c r="L68" s="2">
         <v>38507868</v>
@@ -3111,25 +3115,25 @@
         <v>18</v>
       </c>
       <c r="B69" t="s">
+        <v>165</v>
+      </c>
+      <c r="C69" t="s">
+        <v>31</v>
+      </c>
+      <c r="D69" t="s">
+        <v>34</v>
+      </c>
+      <c r="E69" t="s">
+        <v>170</v>
+      </c>
+      <c r="F69" t="s">
         <v>175</v>
       </c>
-      <c r="C69" t="s">
-        <v>31</v>
-      </c>
-      <c r="D69" t="s">
-        <v>34</v>
-      </c>
-      <c r="E69" t="s">
-        <v>180</v>
-      </c>
-      <c r="F69" t="s">
-        <v>185</v>
-      </c>
       <c r="G69" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="H69" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="L69" s="2">
         <v>38508121</v>
@@ -3144,7 +3148,7 @@
         <v>18</v>
       </c>
       <c r="B70" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C70" t="s">
         <v>31</v>
@@ -3153,16 +3157,16 @@
         <v>34</v>
       </c>
       <c r="E70" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="F70" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="G70" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="H70" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="L70" s="2">
         <v>38508566</v>
@@ -3177,7 +3181,7 @@
         <v>18</v>
       </c>
       <c r="B71" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C71" t="s">
         <v>31</v>
@@ -3186,19 +3190,19 @@
         <v>34</v>
       </c>
       <c r="E71" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="F71" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="G71" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="H71" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="I71" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="L71" s="2">
         <v>38509129</v>
@@ -3213,7 +3217,7 @@
         <v>18</v>
       </c>
       <c r="B72" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C72" t="s">
         <v>31</v>
@@ -3222,7 +3226,7 @@
         <v>34</v>
       </c>
       <c r="E72" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="L72" s="2">
         <v>38509297</v>
@@ -3237,7 +3241,7 @@
         <v>18</v>
       </c>
       <c r="B73" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C73" t="s">
         <v>31</v>
@@ -3246,7 +3250,7 @@
         <v>34</v>
       </c>
       <c r="E73" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="L73" s="2">
         <v>38509325</v>
@@ -3261,7 +3265,7 @@
         <v>14</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C74" s="10"/>
       <c r="D74" s="10" t="s">
@@ -3282,19 +3286,15 @@
       <c r="M74" s="11">
         <v>2709547</v>
       </c>
-      <c r="N74" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="O74" s="10" t="s">
-        <v>124</v>
-      </c>
+      <c r="N74" s="10"/>
+      <c r="O74" s="10"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A75" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C75" s="10"/>
       <c r="D75" s="10" t="s">
@@ -3315,19 +3315,15 @@
       <c r="M75" s="11">
         <v>2709547</v>
       </c>
-      <c r="N75" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="O75" s="10" t="s">
-        <v>124</v>
-      </c>
+      <c r="N75" s="10"/>
+      <c r="O75" s="10"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C76" s="10"/>
       <c r="D76" s="10" t="s">
@@ -3348,19 +3344,15 @@
       <c r="M76" s="11">
         <v>2709547</v>
       </c>
-      <c r="N76" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="O76" s="10" t="s">
-        <v>124</v>
-      </c>
+      <c r="N76" s="10"/>
+      <c r="O76" s="10"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A77" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C77" s="10"/>
       <c r="D77" s="10" t="s">
@@ -3381,12 +3373,8 @@
       <c r="M77" s="11">
         <v>2709547</v>
       </c>
-      <c r="N77" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="O77" s="10" t="s">
-        <v>124</v>
-      </c>
+      <c r="N77" s="10"/>
+      <c r="O77" s="10"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80" s="14"/>

</xml_diff>

<commit_message>
add handling for Neighborly edge case
</commit_message>
<xml_diff>
--- a/Muting Rules.xlsx
+++ b/Muting Rules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://2ndwatch-my.sharepoint.com/personal/aeversmeyer_2ndwatch_com/Documents/Documents/Tooling/NR Muting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeversmeyer\Muting Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="717" documentId="8_{F3C4CCFD-D3A3-4A0C-A232-E9C71F11B485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0463F129-B798-4DF9-9E3B-A1CA3351B187}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AE36F9-E0F5-4282-9724-65A2F3D874BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="470" yWindow="1700" windowWidth="37680" windowHeight="16840" xr2:uid="{D6AE10F8-5FA4-4DCC-834E-28D78D72E9DB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="198">
   <si>
     <t>Environment</t>
   </si>
@@ -627,6 +627,9 @@
   </si>
   <si>
     <t>GreenFirst Forsest Products</t>
+  </si>
+  <si>
+    <t>different times for same event</t>
   </si>
 </sst>
 </file>
@@ -762,10 +765,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1067,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5344475A-C7FB-4B36-9EFD-5513E556E893}">
   <dimension ref="A1:O81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="C29" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45:N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2449,7 +2448,9 @@
       <c r="M45" s="11">
         <v>3446638</v>
       </c>
-      <c r="N45" s="10"/>
+      <c r="N45" s="10" t="s">
+        <v>197</v>
+      </c>
       <c r="O45" s="9" t="s">
         <v>103</v>
       </c>
@@ -2482,7 +2483,9 @@
       <c r="M46" s="11">
         <v>3446638</v>
       </c>
-      <c r="N46" s="10"/>
+      <c r="N46" s="10" t="s">
+        <v>197</v>
+      </c>
       <c r="O46" s="9" t="s">
         <v>103</v>
       </c>
@@ -2515,7 +2518,9 @@
       <c r="M47" s="11">
         <v>3446638</v>
       </c>
-      <c r="N47" s="10"/>
+      <c r="N47" s="10" t="s">
+        <v>197</v>
+      </c>
       <c r="O47" s="9" t="s">
         <v>103</v>
       </c>
@@ -2548,7 +2553,9 @@
       <c r="M48" s="11">
         <v>3446638</v>
       </c>
-      <c r="N48" s="10"/>
+      <c r="N48" s="10" t="s">
+        <v>197</v>
+      </c>
       <c r="O48" s="9" t="s">
         <v>103</v>
       </c>
@@ -2581,7 +2588,9 @@
       <c r="M49" s="11">
         <v>3446638</v>
       </c>
-      <c r="N49" s="10"/>
+      <c r="N49" s="10" t="s">
+        <v>197</v>
+      </c>
       <c r="O49" s="9" t="s">
         <v>103</v>
       </c>

</xml_diff>

<commit_message>
add Lenovo special handling
</commit_message>
<xml_diff>
--- a/Muting Rules.xlsx
+++ b/Muting Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeversmeyer\Muting Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AE36F9-E0F5-4282-9724-65A2F3D874BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C4BF75-411F-493F-84D0-8E69BC8A0499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="470" yWindow="1700" windowWidth="37680" windowHeight="16840" xr2:uid="{D6AE10F8-5FA4-4DCC-834E-28D78D72E9DB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="199">
   <si>
     <t>Environment</t>
   </si>
@@ -605,31 +605,34 @@
     <t>Non-Prod -App, IIS and SQL group3</t>
   </si>
   <si>
-    <t>Non-Prod - ECS</t>
-  </si>
-  <si>
     <t>Prod -App, IIS and SQL group3</t>
   </si>
   <si>
     <t>Prod - App,Prod-Infra Group 1, and SQL group1</t>
   </si>
   <si>
-    <t>Prod -App,Prod -Infra Group 2, and SQL group2</t>
-  </si>
-  <si>
-    <t>Prod - Azure</t>
-  </si>
-  <si>
-    <t>Prod - ECS</t>
-  </si>
-  <si>
     <t>Non-Prod - App and SQL group1</t>
   </si>
   <si>
     <t>GreenFirst Forsest Products</t>
   </si>
   <si>
-    <t>different times for same event</t>
+    <t>different times for same event: first hour</t>
+  </si>
+  <si>
+    <t>different times for same event: last three hours</t>
+  </si>
+  <si>
+    <t>Non-Prod  - ECS</t>
+  </si>
+  <si>
+    <t>Prod -App,Prod -Infra Group 2 and SQL group2</t>
+  </si>
+  <si>
+    <t>Prod  - Azure</t>
+  </si>
+  <si>
+    <t>Prod  - ECS</t>
   </si>
 </sst>
 </file>
@@ -1066,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5344475A-C7FB-4B36-9EFD-5513E556E893}">
   <dimension ref="A1:O81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C29" workbookViewId="0">
-      <selection activeCell="N45" sqref="N45:N49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1571,7 +1574,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C15" t="s">
         <v>31</v>
@@ -1630,7 +1633,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C17" t="s">
         <v>31</v>
@@ -1660,7 +1663,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C18" t="s">
         <v>31</v>
@@ -1694,7 +1697,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C19" t="s">
         <v>31</v>
@@ -1728,7 +1731,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C20" t="s">
         <v>31</v>
@@ -1762,7 +1765,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C21" t="s">
         <v>31</v>
@@ -1788,7 +1791,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C22" t="s">
         <v>31</v>
@@ -2015,7 +2018,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>99</v>
@@ -2048,7 +2051,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>97</v>
@@ -2449,7 +2452,7 @@
         <v>3446638</v>
       </c>
       <c r="N45" s="10" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="O45" s="9" t="s">
         <v>103</v>
@@ -2484,7 +2487,7 @@
         <v>3446638</v>
       </c>
       <c r="N46" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="O46" s="9" t="s">
         <v>103</v>
@@ -2519,7 +2522,7 @@
         <v>3446638</v>
       </c>
       <c r="N47" s="10" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="O47" s="9" t="s">
         <v>103</v>
@@ -2554,7 +2557,7 @@
         <v>3446638</v>
       </c>
       <c r="N48" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="O48" s="9" t="s">
         <v>103</v>
@@ -2588,9 +2591,7 @@
       <c r="M49" s="11">
         <v>3446638</v>
       </c>
-      <c r="N49" s="10" t="s">
-        <v>197</v>
-      </c>
+      <c r="N49" s="10"/>
       <c r="O49" s="9" t="s">
         <v>103</v>
       </c>

</xml_diff>

<commit_message>
handle neighborly spillover exception
</commit_message>
<xml_diff>
--- a/Muting Rules.xlsx
+++ b/Muting Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeversmeyer\Muting Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C4BF75-411F-493F-84D0-8E69BC8A0499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3B907D-3030-49D5-A79F-F1384C8FBE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="470" yWindow="1700" windowWidth="37680" windowHeight="16840" xr2:uid="{D6AE10F8-5FA4-4DCC-834E-28D78D72E9DB}"/>
+    <workbookView xWindow="500" yWindow="2290" windowWidth="37680" windowHeight="16840" xr2:uid="{D6AE10F8-5FA4-4DCC-834E-28D78D72E9DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="202">
   <si>
     <t>Environment</t>
   </si>
@@ -633,6 +633,15 @@
   </si>
   <si>
     <t>Prod  - ECS</t>
+  </si>
+  <si>
+    <t>Verizon</t>
+  </si>
+  <si>
+    <t>Pre-Prod</t>
+  </si>
+  <si>
+    <t>ssm_Pre-Prod</t>
   </si>
 </sst>
 </file>
@@ -725,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -753,6 +762,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1067,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5344475A-C7FB-4B36-9EFD-5513E556E893}">
-  <dimension ref="A1:O81"/>
+  <dimension ref="A1:O83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="L69" sqref="L69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3037,365 +3051,446 @@
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="10"/>
+      <c r="K66" s="10"/>
+      <c r="L66" s="11">
+        <v>39296621</v>
+      </c>
+      <c r="M66" s="11">
+        <v>2401533</v>
+      </c>
+      <c r="N66" s="10"/>
+      <c r="O66" s="10"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A67" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="10"/>
+      <c r="K67" s="10"/>
+      <c r="L67" s="11">
+        <v>39296642</v>
+      </c>
+      <c r="M67" s="11">
+        <v>2401533</v>
+      </c>
+      <c r="N67" s="10"/>
+      <c r="O67" s="10"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A68" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B68" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9" t="s">
+      <c r="C68" s="15"/>
+      <c r="D68" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E66" s="9" t="s">
+      <c r="E68" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-      <c r="H66" s="9"/>
-      <c r="I66" s="9"/>
-      <c r="J66" s="9"/>
-      <c r="K66" s="9"/>
-      <c r="L66" s="11">
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+      <c r="J68" s="15"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="16">
         <v>38422496</v>
       </c>
-      <c r="M66" s="11">
+      <c r="M68" s="16">
         <v>2739512</v>
       </c>
-      <c r="N66" s="9" t="s">
+      <c r="N68" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="O66" s="9"/>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A67" s="4" t="s">
+      <c r="O68" s="15"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A69" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B69" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="C67" t="s">
-        <v>31</v>
-      </c>
-      <c r="D67" t="s">
-        <v>34</v>
-      </c>
-      <c r="E67" t="s">
+      <c r="C69" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E69" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="L67" s="2">
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
+      <c r="J69" s="10"/>
+      <c r="K69" s="10"/>
+      <c r="L69" s="11">
         <v>38507716</v>
       </c>
-      <c r="M67" s="2">
+      <c r="M69" s="11">
         <v>2671646</v>
       </c>
-      <c r="N67"/>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A68" s="4" t="s">
+      <c r="N69" s="10"/>
+      <c r="O69" s="10"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A70" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B70" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="C68" t="s">
-        <v>31</v>
-      </c>
-      <c r="D68" t="s">
-        <v>34</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="C70" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E70" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F70" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G70" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="L68" s="2">
+      <c r="H70" s="10"/>
+      <c r="I70" s="10"/>
+      <c r="J70" s="10"/>
+      <c r="K70" s="10"/>
+      <c r="L70" s="11">
         <v>38507868</v>
       </c>
-      <c r="M68" s="2">
+      <c r="M70" s="11">
         <v>2671646</v>
       </c>
-      <c r="N68"/>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A69" s="4" t="s">
+      <c r="N70" s="10"/>
+      <c r="O70" s="10"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A71" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B71" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="C69" t="s">
-        <v>31</v>
-      </c>
-      <c r="D69" t="s">
-        <v>34</v>
-      </c>
-      <c r="E69" t="s">
+      <c r="C71" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E71" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F71" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G71" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H71" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="L69" s="2">
+      <c r="I71" s="10"/>
+      <c r="J71" s="10"/>
+      <c r="K71" s="10"/>
+      <c r="L71" s="11">
         <v>38508121</v>
       </c>
-      <c r="M69" s="2">
+      <c r="M71" s="11">
         <v>2671646</v>
       </c>
-      <c r="N69"/>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A70" s="4" t="s">
+      <c r="N71" s="10"/>
+      <c r="O71" s="10"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A72" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B72" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="C70" t="s">
-        <v>31</v>
-      </c>
-      <c r="D70" t="s">
-        <v>34</v>
-      </c>
-      <c r="E70" t="s">
+      <c r="C72" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E72" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F72" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G72" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H72" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="L70" s="2">
+      <c r="I72" s="10"/>
+      <c r="J72" s="10"/>
+      <c r="K72" s="10"/>
+      <c r="L72" s="11">
         <v>38508566</v>
       </c>
-      <c r="M70" s="2">
+      <c r="M72" s="11">
         <v>2671646</v>
       </c>
-      <c r="N70"/>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A71" s="4" t="s">
+      <c r="N72" s="10"/>
+      <c r="O72" s="10"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A73" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B73" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="C71" t="s">
-        <v>31</v>
-      </c>
-      <c r="D71" t="s">
-        <v>34</v>
-      </c>
-      <c r="E71" t="s">
+      <c r="C73" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E73" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F73" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G73" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="H71" t="s">
+      <c r="H73" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="I71" t="s">
+      <c r="I73" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="L71" s="2">
+      <c r="J73" s="10"/>
+      <c r="K73" s="10"/>
+      <c r="L73" s="11">
         <v>38509129</v>
       </c>
-      <c r="M71" s="2">
+      <c r="M73" s="11">
         <v>2671646</v>
       </c>
-      <c r="N71"/>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A72" s="4" t="s">
+      <c r="N73" s="10"/>
+      <c r="O73" s="10"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A74" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B74" t="s">
         <v>124</v>
       </c>
-      <c r="C72" t="s">
-        <v>31</v>
-      </c>
-      <c r="D72" t="s">
-        <v>34</v>
-      </c>
-      <c r="E72" t="s">
+      <c r="C74" t="s">
+        <v>31</v>
+      </c>
+      <c r="D74" t="s">
+        <v>34</v>
+      </c>
+      <c r="E74" t="s">
         <v>185</v>
       </c>
-      <c r="L72" s="2">
+      <c r="L74" s="2">
         <v>38509297</v>
       </c>
-      <c r="M72" s="2">
+      <c r="M74" s="2">
         <v>2671646</v>
       </c>
-      <c r="N72"/>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A73" s="4" t="s">
+      <c r="N74"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A75" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B75" t="s">
         <v>163</v>
       </c>
-      <c r="C73" t="s">
-        <v>31</v>
-      </c>
-      <c r="D73" t="s">
-        <v>34</v>
-      </c>
-      <c r="E73" t="s">
+      <c r="C75" t="s">
+        <v>31</v>
+      </c>
+      <c r="D75" t="s">
+        <v>34</v>
+      </c>
+      <c r="E75" t="s">
         <v>186</v>
       </c>
-      <c r="L73" s="2">
+      <c r="L75" s="2">
         <v>38509325</v>
       </c>
-      <c r="M73" s="2">
+      <c r="M75" s="2">
         <v>2671646</v>
       </c>
-      <c r="N73"/>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A74" s="9" t="s">
+      <c r="N75"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A76" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B74" s="10" t="s">
+      <c r="B76" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C74" s="10"/>
-      <c r="D74" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E74" s="10" t="s">
+      <c r="C76" s="17"/>
+      <c r="D76" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E76" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F74" s="10"/>
-      <c r="G74" s="10"/>
-      <c r="H74" s="10"/>
-      <c r="I74" s="10"/>
-      <c r="J74" s="10"/>
-      <c r="K74" s="10"/>
-      <c r="L74" s="11">
+      <c r="F76" s="17"/>
+      <c r="G76" s="17"/>
+      <c r="H76" s="17"/>
+      <c r="I76" s="17"/>
+      <c r="J76" s="17"/>
+      <c r="K76" s="17"/>
+      <c r="L76" s="16">
         <v>38456369</v>
       </c>
-      <c r="M74" s="11">
+      <c r="M76" s="16">
         <v>2709547</v>
       </c>
-      <c r="N74" s="10"/>
-      <c r="O74" s="10"/>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A75" s="9" t="s">
+      <c r="N76" s="17"/>
+      <c r="O76" s="17"/>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A77" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B75" s="10" t="s">
+      <c r="B77" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E75" s="10" t="s">
+      <c r="C77" s="17"/>
+      <c r="D77" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E77" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F75" s="10"/>
-      <c r="G75" s="10"/>
-      <c r="H75" s="10"/>
-      <c r="I75" s="10"/>
-      <c r="J75" s="10"/>
-      <c r="K75" s="10"/>
-      <c r="L75" s="11">
+      <c r="F77" s="17"/>
+      <c r="G77" s="17"/>
+      <c r="H77" s="17"/>
+      <c r="I77" s="17"/>
+      <c r="J77" s="17"/>
+      <c r="K77" s="17"/>
+      <c r="L77" s="16">
         <v>38456394</v>
       </c>
-      <c r="M75" s="11">
+      <c r="M77" s="16">
         <v>2709547</v>
       </c>
-      <c r="N75" s="10"/>
-      <c r="O75" s="10"/>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A76" s="9" t="s">
+      <c r="N77" s="17"/>
+      <c r="O77" s="17"/>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A78" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B76" s="10" t="s">
+      <c r="B78" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E76" s="10" t="s">
+      <c r="C78" s="17"/>
+      <c r="D78" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E78" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F76" s="10"/>
-      <c r="G76" s="10"/>
-      <c r="H76" s="10"/>
-      <c r="I76" s="10"/>
-      <c r="J76" s="10"/>
-      <c r="K76" s="10"/>
-      <c r="L76" s="11">
+      <c r="F78" s="17"/>
+      <c r="G78" s="17"/>
+      <c r="H78" s="17"/>
+      <c r="I78" s="17"/>
+      <c r="J78" s="17"/>
+      <c r="K78" s="17"/>
+      <c r="L78" s="16">
         <v>38456301</v>
       </c>
-      <c r="M76" s="11">
+      <c r="M78" s="16">
         <v>2709547</v>
       </c>
-      <c r="N76" s="10"/>
-      <c r="O76" s="10"/>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A77" s="9" t="s">
+      <c r="N78" s="17"/>
+      <c r="O78" s="17"/>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A79" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B77" s="10" t="s">
+      <c r="B79" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E77" s="10" t="s">
+      <c r="C79" s="17"/>
+      <c r="D79" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E79" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="F77" s="10"/>
-      <c r="G77" s="10"/>
-      <c r="H77" s="10"/>
-      <c r="I77" s="10"/>
-      <c r="J77" s="10"/>
-      <c r="K77" s="10"/>
-      <c r="L77" s="11">
+      <c r="F79" s="17"/>
+      <c r="G79" s="17"/>
+      <c r="H79" s="17"/>
+      <c r="I79" s="17"/>
+      <c r="J79" s="17"/>
+      <c r="K79" s="17"/>
+      <c r="L79" s="16">
         <v>38456341</v>
       </c>
-      <c r="M77" s="11">
+      <c r="M79" s="16">
         <v>2709547</v>
       </c>
-      <c r="N77" s="10"/>
-      <c r="O77" s="10"/>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A80" s="14"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A81" s="4"/>
+      <c r="N79" s="17"/>
+      <c r="O79" s="17"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="14"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O82">
-    <sortCondition ref="A2:A82"/>
-    <sortCondition ref="B2:B82"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O84">
+    <sortCondition ref="A2:A84"/>
+    <sortCondition ref="B2:B84"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change Lazerpro env name
</commit_message>
<xml_diff>
--- a/Muting Rules.xlsx
+++ b/Muting Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeversmeyer\Python\2w-patching-daily-muting-check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C114BF70-AEDE-479A-BC6F-A70B4A3C310E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C0E2C0-F21C-429F-A418-B177C0278621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38910" yWindow="890" windowWidth="36820" windowHeight="19540" xr2:uid="{D6AE10F8-5FA4-4DCC-834E-28D78D72E9DB}"/>
+    <workbookView xWindow="39660" yWindow="1010" windowWidth="36820" windowHeight="19540" xr2:uid="{D6AE10F8-5FA4-4DCC-834E-28D78D72E9DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="198">
   <si>
     <t>Environment</t>
   </si>
@@ -630,9 +630,6 @@
   </si>
   <si>
     <t>ssm_Pre-Prod</t>
-  </si>
-  <si>
-    <t>Prod All</t>
   </si>
 </sst>
 </file>
@@ -1069,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5344475A-C7FB-4B36-9EFD-5513E556E893}">
   <dimension ref="A1:O81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2200,7 +2197,7 @@
         <v>26</v>
       </c>
       <c r="B37" t="s">
-        <v>198</v>
+        <v>95</v>
       </c>
       <c r="D37" t="s">
         <v>33</v>

</xml_diff>